<commit_message>
add rc experiment bash file
</commit_message>
<xml_diff>
--- a/models/dft/rc/properties.xlsx
+++ b/models/dft/rc/properties.xlsx
@@ -341,8 +341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -354,127 +354,127 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1.2</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1.6</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>1.8</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2.2000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2.4</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2.6</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2.8</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>3.2</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>3.4</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>3.6</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>3.8</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>4.2</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>4.4000000000000004</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>4.5999999999999996</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>4.8</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>